<commit_message>
Write Excel Data and maintain ActiTimeTest Data
</commit_message>
<xml_diff>
--- a/wcsm9automationproject/src/main/resources/TestData.xlsx
+++ b/wcsm9automationproject/src/main/resources/TestData.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Team</t>
   </si>
@@ -85,12 +85,19 @@
   </si>
   <si>
     <t>SD</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -452,6 +459,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -531,6 +541,11 @@
       </c>
       <c r="B11" s="2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>